<commit_message>
finished the array1  to array3 transformation
</commit_message>
<xml_diff>
--- a/data/new data/new data.xlsx
+++ b/data/new data/new data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacob/GitHub/drug_pricing/data/new data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01617A9-2809-6C4A-9D92-3A187FE1B47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6B8823-3ED9-BE40-A5F9-5B5B2683B3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Proper Name</t>
   </si>
@@ -155,30 +155,6 @@
   </si>
   <si>
     <t>FY-2038</t>
-  </si>
-  <si>
-    <t>Regeneron Pharmaceuticals</t>
-  </si>
-  <si>
-    <t>Sanofi</t>
-  </si>
-  <si>
-    <t>ExUS</t>
-  </si>
-  <si>
-    <t>Dupixent 1</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>BLA</t>
-  </si>
-  <si>
-    <t>Test drug</t>
-  </si>
-  <si>
-    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -267,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -275,29 +251,28 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -317,7 +292,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -640,13 +615,10 @@
   <dimension ref="A1:AS2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="15.1640625" style="4"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -785,142 +757,52 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="1">
-        <v>480146969.85000002</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="9">
-        <v>42822</v>
-      </c>
-      <c r="M2" s="10">
-        <v>2017</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1">
-        <v>0</v>
-      </c>
-      <c r="V2" s="1">
-        <v>0</v>
-      </c>
-      <c r="W2" s="1">
-        <v>0</v>
-      </c>
-      <c r="X2" s="1">
-        <v>2.5059999999999998</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>145.50049603593388</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>444.39144938234119</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>823.80512579782521</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>1486.850865145597</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>2108.0602061374602</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>2615.9284559873572</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>3032.5680079232934</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>3420.0792176186433</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>3785.6571182420766</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>4165.6717754899337</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>4370.8732097302827</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>4605.9423516272891</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>4595.4204355336587</v>
-      </c>
-      <c r="AL2" s="1">
-        <v>4274.9068749078979</v>
-      </c>
-      <c r="AM2" s="2">
-        <v>3568.9047427437299</v>
-      </c>
-      <c r="AN2" s="2">
-        <v>1758.8299135022348</v>
-      </c>
-      <c r="AO2" s="2">
-        <v>2788.4206419736502</v>
-      </c>
-      <c r="AP2" s="2">
-        <v>2509.5785777762799</v>
-      </c>
-      <c r="AQ2" s="2">
-        <v>2230.73651357892</v>
-      </c>
-      <c r="AR2" s="2">
-        <v>1951.89444938155</v>
-      </c>
-      <c r="AS2" s="2">
-        <v>1673.0523851841901</v>
-      </c>
+    <row r="2" spans="1:45" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>